<commit_message>
Add and Edit Papers
adding templates for making contributions to database
</commit_message>
<xml_diff>
--- a/Process Variables.xlsx
+++ b/Process Variables.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="6860" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="157">
   <si>
     <t>Author</t>
   </si>
@@ -141,9 +141,6 @@
     <t>DipRate</t>
   </si>
   <si>
-    <t>DIpTime</t>
-  </si>
-  <si>
     <t>FilmRange</t>
   </si>
   <si>
@@ -322,13 +319,184 @@
   </si>
   <si>
     <t>ChanLenRange</t>
+  </si>
+  <si>
+    <t>Regioregularity</t>
+  </si>
+  <si>
+    <t>Initial Concentration</t>
+  </si>
+  <si>
+    <t>Solvent 1</t>
+  </si>
+  <si>
+    <t>Volume Fraction Solvent 1</t>
+  </si>
+  <si>
+    <t>Solution Treatment</t>
+  </si>
+  <si>
+    <t>Substrate Treatment</t>
+  </si>
+  <si>
+    <t>Processing Environment</t>
+  </si>
+  <si>
+    <t>Evaporation Control</t>
+  </si>
+  <si>
+    <t>Film Thickness</t>
+  </si>
+  <si>
+    <t>Mobility Environment</t>
+  </si>
+  <si>
+    <t>OFET Regime</t>
+  </si>
+  <si>
+    <t>Channel Length</t>
+  </si>
+  <si>
+    <t>Channel Width</t>
+  </si>
+  <si>
+    <t>Room Temp. Mobility</t>
+  </si>
+  <si>
+    <t>Deposition Method</t>
+  </si>
+  <si>
+    <t>BladeVel</t>
+  </si>
+  <si>
+    <t>BladeH</t>
+  </si>
+  <si>
+    <t>DropSize</t>
+  </si>
+  <si>
+    <t>Droplet Size for Casting</t>
+  </si>
+  <si>
+    <t>Blade Velocity</t>
+  </si>
+  <si>
+    <t>Blade Height</t>
+  </si>
+  <si>
+    <t>mm/s</t>
+  </si>
+  <si>
+    <t>µL</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>Process Variable Abbreviation</t>
+  </si>
+  <si>
+    <t>Full Name</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Categorical names, if applicable</t>
+  </si>
+  <si>
+    <t>Number Average Molecular Weight</t>
+  </si>
+  <si>
+    <t>Weight Average MW</t>
+  </si>
+  <si>
+    <t>Polydispersity Index</t>
+  </si>
+  <si>
+    <t>Solvent 2</t>
+  </si>
+  <si>
+    <t>Boiling Point</t>
+  </si>
+  <si>
+    <t>Hansen Radius</t>
+  </si>
+  <si>
+    <t>Spin Coating Rate</t>
+  </si>
+  <si>
+    <t>Spin Coating Time</t>
+  </si>
+  <si>
+    <t>Dip Coating Rate</t>
+  </si>
+  <si>
+    <t>Dip Coating Time</t>
+  </si>
+  <si>
+    <t>DipTime</t>
+  </si>
+  <si>
+    <t>Range of Film Thicknesses</t>
+  </si>
+  <si>
+    <t>Annealing Temperature</t>
+  </si>
+  <si>
+    <t>Annealing Time</t>
+  </si>
+  <si>
+    <t>Annealing Cooling</t>
+  </si>
+  <si>
+    <t>OFET Electrode Configuration</t>
+  </si>
+  <si>
+    <t>Drain-Source Voltage used for transfer curve</t>
+  </si>
+  <si>
+    <t>Nozzle Displacement</t>
+  </si>
+  <si>
+    <t>Spray Time</t>
+  </si>
+  <si>
+    <t>Electrode Material</t>
+  </si>
+  <si>
+    <t>Sonication Time</t>
+  </si>
+  <si>
+    <t>Casting Conditions</t>
+  </si>
+  <si>
+    <t>On/Off Ratio</t>
+  </si>
+  <si>
+    <t>Threshold Voltage</t>
+  </si>
+  <si>
+    <t>HMDS</t>
+  </si>
+  <si>
+    <t>OTS</t>
+  </si>
+  <si>
+    <t>FDTS</t>
+  </si>
+  <si>
+    <t>Solution Aging Time</t>
+  </si>
+  <si>
+    <t>Solution Aging Temperature</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -342,8 +510,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -364,12 +540,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -383,18 +553,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,10 +576,10 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,462 +919,652 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P49"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="17.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
+      <c r="C2" s="7"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="7"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:17">
+      <c r="A6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="8"/>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:17">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:17">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:17">
+      <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" t="s">
+      <c r="B10" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
         <v>55</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F10" t="s">
         <v>56</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G10" t="s">
         <v>57</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H10" t="s">
         <v>58</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I10" t="s">
         <v>59</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J10" t="s">
         <v>60</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K10" t="s">
         <v>61</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L10" t="s">
         <v>62</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M10" t="s">
         <v>63</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N10" t="s">
         <v>64</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O10" t="s">
+        <v>95</v>
+      </c>
+      <c r="P10" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="7"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="7"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" t="s">
+        <v>152</v>
+      </c>
+      <c r="E18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" t="s">
         <v>65</v>
       </c>
-      <c r="N9" t="s">
-        <v>96</v>
-      </c>
-      <c r="O9" t="s">
-        <v>97</v>
-      </c>
-      <c r="P9" t="s">
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" t="s">
+        <v>67</v>
+      </c>
+      <c r="F33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="7"/>
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E35" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" t="s">
+        <v>75</v>
+      </c>
+      <c r="G35" t="s">
+        <v>76</v>
+      </c>
+      <c r="H35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="5" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" t="s">
-        <v>66</v>
-      </c>
-      <c r="D29" t="s">
-        <v>68</v>
-      </c>
-      <c r="E29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" t="s">
-        <v>74</v>
-      </c>
-      <c r="D31" t="s">
-        <v>75</v>
-      </c>
-      <c r="E31" t="s">
-        <v>76</v>
-      </c>
-      <c r="F31" t="s">
-        <v>77</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="B42" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" s="6" t="s">
+      <c r="E42" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B43" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C43" s="7"/>
+      <c r="D43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E43" t="s">
+        <v>81</v>
+      </c>
+      <c r="F43" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" t="s">
+        <v>83</v>
+      </c>
+      <c r="H43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="7"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="6" t="s">
+    <row r="48" spans="1:8">
+      <c r="A48" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C48" s="7"/>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B39" s="8"/>
-      <c r="C39" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" t="s">
-        <v>82</v>
-      </c>
-      <c r="E39" t="s">
-        <v>83</v>
-      </c>
-      <c r="F39" t="s">
-        <v>84</v>
-      </c>
-      <c r="G39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" s="8"/>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="9"/>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="8"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B45" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B46" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B47" s="8"/>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" s="6"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="6"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="7"/>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>